<commit_message>
feat(employees): add endDate field to employee-related entities and DTOs
</commit_message>
<xml_diff>
--- a/public/template/employee.xlsx
+++ b/public/template/employee.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/defrindr/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/projects/ckb/doorlock-workspace/backend/public/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{291ABDA3-FC6D-894C-A685-39E88E5F5ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADFE41B-9A74-3543-A1EA-07364488EE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{0466D2B5-5C93-5447-8339-B2A5712A7543}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17140" xr2:uid="{0466D2B5-5C93-5447-8339-B2A5712A7543}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>EmployeeNumber</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Dummy User 2</t>
+  </si>
+  <si>
+    <t>EndDate</t>
   </si>
 </sst>
 </file>
@@ -532,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{768F174A-463E-B946-AF5D-2CC3468BCD75}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -554,7 +557,7 @@
     <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -577,22 +580,25 @@
         <v>6</v>
       </c>
       <c r="H1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -614,23 +620,26 @@
       <c r="G2" s="4">
         <v>45658</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="4">
+        <v>45658</v>
+      </c>
+      <c r="I2" s="1">
         <v>0</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -652,19 +661,22 @@
       <c r="G3" s="4">
         <v>45658</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="4">
+        <v>45658</v>
+      </c>
+      <c r="I3" s="1">
         <v>0</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>